<commit_message>
Added Sprint 5 Materials Including Sprint Review and Burndown chart.
</commit_message>
<xml_diff>
--- a/Sprint 5/BurnDownChart_Sprint5.xlsx
+++ b/Sprint 5/BurnDownChart_Sprint5.xlsx
@@ -347,11 +347,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="68271488"/>
-        <c:axId val="135285376"/>
+        <c:axId val="182616832"/>
+        <c:axId val="182620160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68271488"/>
+        <c:axId val="182616832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135285376"/>
+        <c:crossAx val="182620160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135285376"/>
+        <c:axId val="182620160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68271488"/>
+        <c:crossAx val="182616832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -821,43 +821,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,8 +878,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="135038464"/>
-        <c:axId val="135040384"/>
+        <c:axId val="182667904"/>
+        <c:axId val="182686464"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -971,43 +971,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1029,11 +1029,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135038464"/>
-        <c:axId val="135040384"/>
+        <c:axId val="182667904"/>
+        <c:axId val="182686464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135038464"/>
+        <c:axId val="182667904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135040384"/>
+        <c:crossAx val="182686464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135040384"/>
+        <c:axId val="182686464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1204,7 +1204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135038464"/>
+        <c:crossAx val="182667904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2870,7 +2870,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,7 +2885,7 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2944,11 +2944,11 @@
       </c>
       <c r="E6">
         <f>F6-SUM($B6:$C6)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <f>$B$1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2967,11 +2967,11 @@
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E18" si="1">E6-SUM($B7:$C7)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f t="shared" ref="F7:F18" si="2">$B$1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,11 +2990,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3013,11 +3013,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,11 +3036,11 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3059,11 +3059,11 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,11 +3082,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3105,11 +3105,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>9 - 04/21/15</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3128,11 +3128,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4.8</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3151,11 +3151,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4.8</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>11 - 04/23/15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -3174,11 +3174,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3187,21 +3187,21 @@
         <v>12 - 04/24/15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D17">
         <v>12</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>3.5</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3210,21 +3210,21 @@
         <v>13 - 04/25/15</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D18">
         <v>13</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>